<commit_message>
minor fixes. graph updates.
</commit_message>
<xml_diff>
--- a/raw/AT_hospital_data.xlsx
+++ b/raw/AT_hospital_data.xlsx
@@ -105,8 +105,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K503" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K503"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K513" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K513"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Datum"/>
     <tableColumn id="2" name="B"/>
@@ -125,8 +125,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K454" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K454"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K464" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K464"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Datum"/>
     <tableColumn id="2" name="B"/>
@@ -145,8 +145,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:K474" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K474"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:K484" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K484"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Datum"/>
     <tableColumn id="2" name="B"/>
@@ -165,8 +165,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:K474" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K474"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:K484" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K484"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Datum"/>
     <tableColumn id="2" name="B"/>
@@ -185,8 +185,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:K467" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K467"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:K477" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K477"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Datum"/>
     <tableColumn id="2" name="B"/>
@@ -205,8 +205,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:K489" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K489"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:K499" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:K499"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Datum"/>
     <tableColumn id="2" name="B"/>
@@ -18116,6 +18116,356 @@
         <v>647312</v>
       </c>
     </row>
+    <row r="504">
+      <c r="A504" s="1" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B504" t="n">
+        <v>18119</v>
+      </c>
+      <c r="C504" t="n">
+        <v>40162</v>
+      </c>
+      <c r="D504" t="n">
+        <v>108820</v>
+      </c>
+      <c r="E504" t="n">
+        <v>117121</v>
+      </c>
+      <c r="F504" t="n">
+        <v>50223</v>
+      </c>
+      <c r="G504" t="n">
+        <v>80089</v>
+      </c>
+      <c r="H504" t="n">
+        <v>63375</v>
+      </c>
+      <c r="I504" t="n">
+        <v>30223</v>
+      </c>
+      <c r="J504" t="n">
+        <v>139374</v>
+      </c>
+      <c r="K504" t="n">
+        <v>647506</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="1" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B505" t="n">
+        <v>18120</v>
+      </c>
+      <c r="C505" t="n">
+        <v>40178</v>
+      </c>
+      <c r="D505" t="n">
+        <v>108843</v>
+      </c>
+      <c r="E505" t="n">
+        <v>117143</v>
+      </c>
+      <c r="F505" t="n">
+        <v>50228</v>
+      </c>
+      <c r="G505" t="n">
+        <v>80123</v>
+      </c>
+      <c r="H505" t="n">
+        <v>63403</v>
+      </c>
+      <c r="I505" t="n">
+        <v>30223</v>
+      </c>
+      <c r="J505" t="n">
+        <v>139397</v>
+      </c>
+      <c r="K505" t="n">
+        <v>647658</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="1" t="n">
+        <v>44391</v>
+      </c>
+      <c r="B506" t="n">
+        <v>18119</v>
+      </c>
+      <c r="C506" t="n">
+        <v>40228</v>
+      </c>
+      <c r="D506" t="n">
+        <v>108878</v>
+      </c>
+      <c r="E506" t="n">
+        <v>117182</v>
+      </c>
+      <c r="F506" t="n">
+        <v>50246</v>
+      </c>
+      <c r="G506" t="n">
+        <v>80154</v>
+      </c>
+      <c r="H506" t="n">
+        <v>63426</v>
+      </c>
+      <c r="I506" t="n">
+        <v>30233</v>
+      </c>
+      <c r="J506" t="n">
+        <v>139477</v>
+      </c>
+      <c r="K506" t="n">
+        <v>647943</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="1" t="n">
+        <v>44392</v>
+      </c>
+      <c r="B507" t="n">
+        <v>18127</v>
+      </c>
+      <c r="C507" t="n">
+        <v>40253</v>
+      </c>
+      <c r="D507" t="n">
+        <v>108929</v>
+      </c>
+      <c r="E507" t="n">
+        <v>117222</v>
+      </c>
+      <c r="F507" t="n">
+        <v>50273</v>
+      </c>
+      <c r="G507" t="n">
+        <v>80179</v>
+      </c>
+      <c r="H507" t="n">
+        <v>63444</v>
+      </c>
+      <c r="I507" t="n">
+        <v>30247</v>
+      </c>
+      <c r="J507" t="n">
+        <v>139649</v>
+      </c>
+      <c r="K507" t="n">
+        <v>648323</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="1" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B508" t="n">
+        <v>18129</v>
+      </c>
+      <c r="C508" t="n">
+        <v>40268</v>
+      </c>
+      <c r="D508" t="n">
+        <v>108951</v>
+      </c>
+      <c r="E508" t="n">
+        <v>117272</v>
+      </c>
+      <c r="F508" t="n">
+        <v>50311</v>
+      </c>
+      <c r="G508" t="n">
+        <v>80219</v>
+      </c>
+      <c r="H508" t="n">
+        <v>63480</v>
+      </c>
+      <c r="I508" t="n">
+        <v>30256</v>
+      </c>
+      <c r="J508" t="n">
+        <v>139760</v>
+      </c>
+      <c r="K508" t="n">
+        <v>648646</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="1" t="n">
+        <v>44394</v>
+      </c>
+      <c r="B509" t="n">
+        <v>18134</v>
+      </c>
+      <c r="C509" t="n">
+        <v>40279</v>
+      </c>
+      <c r="D509" t="n">
+        <v>109010</v>
+      </c>
+      <c r="E509" t="n">
+        <v>117342</v>
+      </c>
+      <c r="F509" t="n">
+        <v>50374</v>
+      </c>
+      <c r="G509" t="n">
+        <v>80269</v>
+      </c>
+      <c r="H509" t="n">
+        <v>63522</v>
+      </c>
+      <c r="I509" t="n">
+        <v>30281</v>
+      </c>
+      <c r="J509" t="n">
+        <v>139831</v>
+      </c>
+      <c r="K509" t="n">
+        <v>649042</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="1" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B510" t="n">
+        <v>18135</v>
+      </c>
+      <c r="C510" t="n">
+        <v>40290</v>
+      </c>
+      <c r="D510" t="n">
+        <v>109047</v>
+      </c>
+      <c r="E510" t="n">
+        <v>117383</v>
+      </c>
+      <c r="F510" t="n">
+        <v>50418</v>
+      </c>
+      <c r="G510" t="n">
+        <v>80325</v>
+      </c>
+      <c r="H510" t="n">
+        <v>63535</v>
+      </c>
+      <c r="I510" t="n">
+        <v>30297</v>
+      </c>
+      <c r="J510" t="n">
+        <v>139967</v>
+      </c>
+      <c r="K510" t="n">
+        <v>649397</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="1" t="n">
+        <v>44396</v>
+      </c>
+      <c r="B511" t="n">
+        <v>18136</v>
+      </c>
+      <c r="C511" t="n">
+        <v>40301</v>
+      </c>
+      <c r="D511" t="n">
+        <v>109075</v>
+      </c>
+      <c r="E511" t="n">
+        <v>117419</v>
+      </c>
+      <c r="F511" t="n">
+        <v>50435</v>
+      </c>
+      <c r="G511" t="n">
+        <v>80359</v>
+      </c>
+      <c r="H511" t="n">
+        <v>63557</v>
+      </c>
+      <c r="I511" t="n">
+        <v>30318</v>
+      </c>
+      <c r="J511" t="n">
+        <v>140053</v>
+      </c>
+      <c r="K511" t="n">
+        <v>649653</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="1" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B512" t="n">
+        <v>18139</v>
+      </c>
+      <c r="C512" t="n">
+        <v>40317</v>
+      </c>
+      <c r="D512" t="n">
+        <v>109107</v>
+      </c>
+      <c r="E512" t="n">
+        <v>117463</v>
+      </c>
+      <c r="F512" t="n">
+        <v>50521</v>
+      </c>
+      <c r="G512" t="n">
+        <v>80386</v>
+      </c>
+      <c r="H512" t="n">
+        <v>63585</v>
+      </c>
+      <c r="I512" t="n">
+        <v>30342</v>
+      </c>
+      <c r="J512" t="n">
+        <v>140139</v>
+      </c>
+      <c r="K512" t="n">
+        <v>649999</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="1" t="n">
+        <v>44398</v>
+      </c>
+      <c r="B513" t="n">
+        <v>18149</v>
+      </c>
+      <c r="C513" t="n">
+        <v>40343</v>
+      </c>
+      <c r="D513" t="n">
+        <v>109129</v>
+      </c>
+      <c r="E513" t="n">
+        <v>117542</v>
+      </c>
+      <c r="F513" t="n">
+        <v>50587</v>
+      </c>
+      <c r="G513" t="n">
+        <v>80421</v>
+      </c>
+      <c r="H513" t="n">
+        <v>63617</v>
+      </c>
+      <c r="I513" t="n">
+        <v>30370</v>
+      </c>
+      <c r="J513" t="n">
+        <v>140231</v>
+      </c>
+      <c r="K513" t="n">
+        <v>650389</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -34025,6 +34375,356 @@
         <v>13363128</v>
       </c>
     </row>
+    <row r="455">
+      <c r="A455" s="1" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B455" t="n">
+        <v>237779</v>
+      </c>
+      <c r="C455" t="n">
+        <v>320939</v>
+      </c>
+      <c r="D455" t="n">
+        <v>2023332</v>
+      </c>
+      <c r="E455" t="n">
+        <v>757835</v>
+      </c>
+      <c r="F455" t="n">
+        <v>416589</v>
+      </c>
+      <c r="G455" t="n">
+        <v>778071</v>
+      </c>
+      <c r="H455" t="n">
+        <v>998904</v>
+      </c>
+      <c r="I455" t="n">
+        <v>266636</v>
+      </c>
+      <c r="J455" t="n">
+        <v>7616472</v>
+      </c>
+      <c r="K455" t="n">
+        <v>13416557</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="1" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B456" t="n">
+        <v>237929</v>
+      </c>
+      <c r="C456" t="n">
+        <v>321139</v>
+      </c>
+      <c r="D456" t="n">
+        <v>2026280</v>
+      </c>
+      <c r="E456" t="n">
+        <v>758434</v>
+      </c>
+      <c r="F456" t="n">
+        <v>417375</v>
+      </c>
+      <c r="G456" t="n">
+        <v>779339</v>
+      </c>
+      <c r="H456" t="n">
+        <v>999697</v>
+      </c>
+      <c r="I456" t="n">
+        <v>266697</v>
+      </c>
+      <c r="J456" t="n">
+        <v>7670876</v>
+      </c>
+      <c r="K456" t="n">
+        <v>13477766</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="1" t="n">
+        <v>44391</v>
+      </c>
+      <c r="B457" t="n">
+        <v>238406</v>
+      </c>
+      <c r="C457" t="n">
+        <v>321263</v>
+      </c>
+      <c r="D457" t="n">
+        <v>2028591</v>
+      </c>
+      <c r="E457" t="n">
+        <v>759078</v>
+      </c>
+      <c r="F457" t="n">
+        <v>418233</v>
+      </c>
+      <c r="G457" t="n">
+        <v>780031</v>
+      </c>
+      <c r="H457" t="n">
+        <v>1000687</v>
+      </c>
+      <c r="I457" t="n">
+        <v>266788</v>
+      </c>
+      <c r="J457" t="n">
+        <v>7736770</v>
+      </c>
+      <c r="K457" t="n">
+        <v>13549847</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="1" t="n">
+        <v>44392</v>
+      </c>
+      <c r="B458" t="n">
+        <v>238679</v>
+      </c>
+      <c r="C458" t="n">
+        <v>321788</v>
+      </c>
+      <c r="D458" t="n">
+        <v>2031797</v>
+      </c>
+      <c r="E458" t="n">
+        <v>759649</v>
+      </c>
+      <c r="F458" t="n">
+        <v>419082</v>
+      </c>
+      <c r="G458" t="n">
+        <v>780724</v>
+      </c>
+      <c r="H458" t="n">
+        <v>1001563</v>
+      </c>
+      <c r="I458" t="n">
+        <v>266871</v>
+      </c>
+      <c r="J458" t="n">
+        <v>7755339</v>
+      </c>
+      <c r="K458" t="n">
+        <v>13575492</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="1" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B459" t="n">
+        <v>238833</v>
+      </c>
+      <c r="C459" t="n">
+        <v>322095</v>
+      </c>
+      <c r="D459" t="n">
+        <v>2034859</v>
+      </c>
+      <c r="E459" t="n">
+        <v>760236</v>
+      </c>
+      <c r="F459" t="n">
+        <v>420085</v>
+      </c>
+      <c r="G459" t="n">
+        <v>781603</v>
+      </c>
+      <c r="H459" t="n">
+        <v>1002424</v>
+      </c>
+      <c r="I459" t="n">
+        <v>266961</v>
+      </c>
+      <c r="J459" t="n">
+        <v>7843307</v>
+      </c>
+      <c r="K459" t="n">
+        <v>13670403</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="1" t="n">
+        <v>44394</v>
+      </c>
+      <c r="B460" t="n">
+        <v>238865</v>
+      </c>
+      <c r="C460" t="n">
+        <v>322224</v>
+      </c>
+      <c r="D460" t="n">
+        <v>2037920</v>
+      </c>
+      <c r="E460" t="n">
+        <v>760937</v>
+      </c>
+      <c r="F460" t="n">
+        <v>420576</v>
+      </c>
+      <c r="G460" t="n">
+        <v>782031</v>
+      </c>
+      <c r="H460" t="n">
+        <v>1003518</v>
+      </c>
+      <c r="I460" t="n">
+        <v>267087</v>
+      </c>
+      <c r="J460" t="n">
+        <v>7904335</v>
+      </c>
+      <c r="K460" t="n">
+        <v>13737493</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="1" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B461" t="n">
+        <v>239012</v>
+      </c>
+      <c r="C461" t="n">
+        <v>322307</v>
+      </c>
+      <c r="D461" t="n">
+        <v>2040908</v>
+      </c>
+      <c r="E461" t="n">
+        <v>761338</v>
+      </c>
+      <c r="F461" t="n">
+        <v>420935</v>
+      </c>
+      <c r="G461" t="n">
+        <v>782535</v>
+      </c>
+      <c r="H461" t="n">
+        <v>1004294</v>
+      </c>
+      <c r="I461" t="n">
+        <v>267196</v>
+      </c>
+      <c r="J461" t="n">
+        <v>7942197</v>
+      </c>
+      <c r="K461" t="n">
+        <v>13780722</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="1" t="n">
+        <v>44396</v>
+      </c>
+      <c r="B462" t="n">
+        <v>239217</v>
+      </c>
+      <c r="C462" t="n">
+        <v>322497</v>
+      </c>
+      <c r="D462" t="n">
+        <v>2043991</v>
+      </c>
+      <c r="E462" t="n">
+        <v>761991</v>
+      </c>
+      <c r="F462" t="n">
+        <v>421279</v>
+      </c>
+      <c r="G462" t="n">
+        <v>783299</v>
+      </c>
+      <c r="H462" t="n">
+        <v>1005022</v>
+      </c>
+      <c r="I462" t="n">
+        <v>267277</v>
+      </c>
+      <c r="J462" t="n">
+        <v>7971622</v>
+      </c>
+      <c r="K462" t="n">
+        <v>13816195</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="1" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B463" t="n">
+        <v>239366</v>
+      </c>
+      <c r="C463" t="n">
+        <v>322736</v>
+      </c>
+      <c r="D463" t="n">
+        <v>2047121</v>
+      </c>
+      <c r="E463" t="n">
+        <v>762746</v>
+      </c>
+      <c r="F463" t="n">
+        <v>422454</v>
+      </c>
+      <c r="G463" t="n">
+        <v>785246</v>
+      </c>
+      <c r="H463" t="n">
+        <v>1005963</v>
+      </c>
+      <c r="I463" t="n">
+        <v>267443</v>
+      </c>
+      <c r="J463" t="n">
+        <v>8030815</v>
+      </c>
+      <c r="K463" t="n">
+        <v>13883890</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="1" t="n">
+        <v>44398</v>
+      </c>
+      <c r="B464" t="n">
+        <v>239691</v>
+      </c>
+      <c r="C464" t="n">
+        <v>323024</v>
+      </c>
+      <c r="D464" t="n">
+        <v>2049451</v>
+      </c>
+      <c r="E464" t="n">
+        <v>763542</v>
+      </c>
+      <c r="F464" t="n">
+        <v>423395</v>
+      </c>
+      <c r="G464" t="n">
+        <v>786181</v>
+      </c>
+      <c r="H464" t="n">
+        <v>1007018</v>
+      </c>
+      <c r="I464" t="n">
+        <v>267443</v>
+      </c>
+      <c r="J464" t="n">
+        <v>8089772</v>
+      </c>
+      <c r="K464" t="n">
+        <v>13949517</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -50634,6 +51334,356 @@
         <v>102</v>
       </c>
     </row>
+    <row r="475">
+      <c r="A475" s="1" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B475" t="n">
+        <v>4</v>
+      </c>
+      <c r="C475" t="n">
+        <v>12</v>
+      </c>
+      <c r="D475" t="n">
+        <v>18</v>
+      </c>
+      <c r="E475" t="n">
+        <v>6</v>
+      </c>
+      <c r="F475" t="n">
+        <v>3</v>
+      </c>
+      <c r="G475" t="n">
+        <v>2</v>
+      </c>
+      <c r="H475" t="n">
+        <v>5</v>
+      </c>
+      <c r="I475" t="n">
+        <v>1</v>
+      </c>
+      <c r="J475" t="n">
+        <v>52</v>
+      </c>
+      <c r="K475" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B476" t="n">
+        <v>2</v>
+      </c>
+      <c r="C476" t="n">
+        <v>12</v>
+      </c>
+      <c r="D476" t="n">
+        <v>20</v>
+      </c>
+      <c r="E476" t="n">
+        <v>11</v>
+      </c>
+      <c r="F476" t="n">
+        <v>3</v>
+      </c>
+      <c r="G476" t="n">
+        <v>2</v>
+      </c>
+      <c r="H476" t="n">
+        <v>6</v>
+      </c>
+      <c r="I476" t="n">
+        <v>1</v>
+      </c>
+      <c r="J476" t="n">
+        <v>54</v>
+      </c>
+      <c r="K476" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1" t="n">
+        <v>44391</v>
+      </c>
+      <c r="B477" t="n">
+        <v>2</v>
+      </c>
+      <c r="C477" t="n">
+        <v>16</v>
+      </c>
+      <c r="D477" t="n">
+        <v>24</v>
+      </c>
+      <c r="E477" t="n">
+        <v>8</v>
+      </c>
+      <c r="F477" t="n">
+        <v>4</v>
+      </c>
+      <c r="G477" t="n">
+        <v>3</v>
+      </c>
+      <c r="H477" t="n">
+        <v>5</v>
+      </c>
+      <c r="I477" t="n">
+        <v>0</v>
+      </c>
+      <c r="J477" t="n">
+        <v>52</v>
+      </c>
+      <c r="K477" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="1" t="n">
+        <v>44392</v>
+      </c>
+      <c r="B478" t="n">
+        <v>1</v>
+      </c>
+      <c r="C478" t="n">
+        <v>16</v>
+      </c>
+      <c r="D478" t="n">
+        <v>21</v>
+      </c>
+      <c r="E478" t="n">
+        <v>8</v>
+      </c>
+      <c r="F478" t="n">
+        <v>2</v>
+      </c>
+      <c r="G478" t="n">
+        <v>4</v>
+      </c>
+      <c r="H478" t="n">
+        <v>3</v>
+      </c>
+      <c r="I478" t="n">
+        <v>0</v>
+      </c>
+      <c r="J478" t="n">
+        <v>54</v>
+      </c>
+      <c r="K478" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="1" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B479" t="n">
+        <v>1</v>
+      </c>
+      <c r="C479" t="n">
+        <v>14</v>
+      </c>
+      <c r="D479" t="n">
+        <v>19</v>
+      </c>
+      <c r="E479" t="n">
+        <v>7</v>
+      </c>
+      <c r="F479" t="n">
+        <v>2</v>
+      </c>
+      <c r="G479" t="n">
+        <v>6</v>
+      </c>
+      <c r="H479" t="n">
+        <v>4</v>
+      </c>
+      <c r="I479" t="n">
+        <v>0</v>
+      </c>
+      <c r="J479" t="n">
+        <v>52</v>
+      </c>
+      <c r="K479" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="1" t="n">
+        <v>44394</v>
+      </c>
+      <c r="B480" t="n">
+        <v>2</v>
+      </c>
+      <c r="C480" t="n">
+        <v>14</v>
+      </c>
+      <c r="D480" t="n">
+        <v>19</v>
+      </c>
+      <c r="E480" t="n">
+        <v>7</v>
+      </c>
+      <c r="F480" t="n">
+        <v>3</v>
+      </c>
+      <c r="G480" t="n">
+        <v>7</v>
+      </c>
+      <c r="H480" t="n">
+        <v>4</v>
+      </c>
+      <c r="I480" t="n">
+        <v>0</v>
+      </c>
+      <c r="J480" t="n">
+        <v>58</v>
+      </c>
+      <c r="K480" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="1" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B481" t="n">
+        <v>2</v>
+      </c>
+      <c r="C481" t="n">
+        <v>14</v>
+      </c>
+      <c r="D481" t="n">
+        <v>16</v>
+      </c>
+      <c r="E481" t="n">
+        <v>7</v>
+      </c>
+      <c r="F481" t="n">
+        <v>3</v>
+      </c>
+      <c r="G481" t="n">
+        <v>7</v>
+      </c>
+      <c r="H481" t="n">
+        <v>4</v>
+      </c>
+      <c r="I481" t="n">
+        <v>0</v>
+      </c>
+      <c r="J481" t="n">
+        <v>54</v>
+      </c>
+      <c r="K481" t="n">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="1" t="n">
+        <v>44396</v>
+      </c>
+      <c r="B482" t="n">
+        <v>2</v>
+      </c>
+      <c r="C482" t="n">
+        <v>12</v>
+      </c>
+      <c r="D482" t="n">
+        <v>15</v>
+      </c>
+      <c r="E482" t="n">
+        <v>6</v>
+      </c>
+      <c r="F482" t="n">
+        <v>3</v>
+      </c>
+      <c r="G482" t="n">
+        <v>7</v>
+      </c>
+      <c r="H482" t="n">
+        <v>4</v>
+      </c>
+      <c r="I482" t="n">
+        <v>0</v>
+      </c>
+      <c r="J482" t="n">
+        <v>61</v>
+      </c>
+      <c r="K482" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="1" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B483" t="n">
+        <v>3</v>
+      </c>
+      <c r="C483" t="n">
+        <v>9</v>
+      </c>
+      <c r="D483" t="n">
+        <v>15</v>
+      </c>
+      <c r="E483" t="n">
+        <v>7</v>
+      </c>
+      <c r="F483" t="n">
+        <v>2</v>
+      </c>
+      <c r="G483" t="n">
+        <v>6</v>
+      </c>
+      <c r="H483" t="n">
+        <v>6</v>
+      </c>
+      <c r="I483" t="n">
+        <v>1</v>
+      </c>
+      <c r="J483" t="n">
+        <v>75</v>
+      </c>
+      <c r="K483" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="1" t="n">
+        <v>44398</v>
+      </c>
+      <c r="B484" t="n">
+        <v>2</v>
+      </c>
+      <c r="C484" t="n">
+        <v>13</v>
+      </c>
+      <c r="D484" t="n">
+        <v>17</v>
+      </c>
+      <c r="E484" t="n">
+        <v>4</v>
+      </c>
+      <c r="F484" t="n">
+        <v>2</v>
+      </c>
+      <c r="G484" t="n">
+        <v>7</v>
+      </c>
+      <c r="H484" t="n">
+        <v>4</v>
+      </c>
+      <c r="I484" t="n">
+        <v>1</v>
+      </c>
+      <c r="J484" t="n">
+        <v>61</v>
+      </c>
+      <c r="K484" t="n">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -67243,6 +68293,356 @@
         <v>39</v>
       </c>
     </row>
+    <row r="475">
+      <c r="A475" s="1" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B475" t="n">
+        <v>1</v>
+      </c>
+      <c r="C475" t="n">
+        <v>2</v>
+      </c>
+      <c r="D475" t="n">
+        <v>9</v>
+      </c>
+      <c r="E475" t="n">
+        <v>3</v>
+      </c>
+      <c r="F475" t="n">
+        <v>0</v>
+      </c>
+      <c r="G475" t="n">
+        <v>1</v>
+      </c>
+      <c r="H475" t="n">
+        <v>2</v>
+      </c>
+      <c r="I475" t="n">
+        <v>1</v>
+      </c>
+      <c r="J475" t="n">
+        <v>16</v>
+      </c>
+      <c r="K475" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B476" t="n">
+        <v>1</v>
+      </c>
+      <c r="C476" t="n">
+        <v>2</v>
+      </c>
+      <c r="D476" t="n">
+        <v>9</v>
+      </c>
+      <c r="E476" t="n">
+        <v>2</v>
+      </c>
+      <c r="F476" t="n">
+        <v>0</v>
+      </c>
+      <c r="G476" t="n">
+        <v>1</v>
+      </c>
+      <c r="H476" t="n">
+        <v>2</v>
+      </c>
+      <c r="I476" t="n">
+        <v>1</v>
+      </c>
+      <c r="J476" t="n">
+        <v>21</v>
+      </c>
+      <c r="K476" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1" t="n">
+        <v>44391</v>
+      </c>
+      <c r="B477" t="n">
+        <v>0</v>
+      </c>
+      <c r="C477" t="n">
+        <v>2</v>
+      </c>
+      <c r="D477" t="n">
+        <v>9</v>
+      </c>
+      <c r="E477" t="n">
+        <v>2</v>
+      </c>
+      <c r="F477" t="n">
+        <v>0</v>
+      </c>
+      <c r="G477" t="n">
+        <v>1</v>
+      </c>
+      <c r="H477" t="n">
+        <v>1</v>
+      </c>
+      <c r="I477" t="n">
+        <v>0</v>
+      </c>
+      <c r="J477" t="n">
+        <v>18</v>
+      </c>
+      <c r="K477" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="1" t="n">
+        <v>44392</v>
+      </c>
+      <c r="B478" t="n">
+        <v>0</v>
+      </c>
+      <c r="C478" t="n">
+        <v>2</v>
+      </c>
+      <c r="D478" t="n">
+        <v>9</v>
+      </c>
+      <c r="E478" t="n">
+        <v>2</v>
+      </c>
+      <c r="F478" t="n">
+        <v>0</v>
+      </c>
+      <c r="G478" t="n">
+        <v>1</v>
+      </c>
+      <c r="H478" t="n">
+        <v>0</v>
+      </c>
+      <c r="I478" t="n">
+        <v>0</v>
+      </c>
+      <c r="J478" t="n">
+        <v>19</v>
+      </c>
+      <c r="K478" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="1" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B479" t="n">
+        <v>0</v>
+      </c>
+      <c r="C479" t="n">
+        <v>2</v>
+      </c>
+      <c r="D479" t="n">
+        <v>9</v>
+      </c>
+      <c r="E479" t="n">
+        <v>2</v>
+      </c>
+      <c r="F479" t="n">
+        <v>0</v>
+      </c>
+      <c r="G479" t="n">
+        <v>2</v>
+      </c>
+      <c r="H479" t="n">
+        <v>1</v>
+      </c>
+      <c r="I479" t="n">
+        <v>0</v>
+      </c>
+      <c r="J479" t="n">
+        <v>21</v>
+      </c>
+      <c r="K479" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="1" t="n">
+        <v>44394</v>
+      </c>
+      <c r="B480" t="n">
+        <v>0</v>
+      </c>
+      <c r="C480" t="n">
+        <v>2</v>
+      </c>
+      <c r="D480" t="n">
+        <v>7</v>
+      </c>
+      <c r="E480" t="n">
+        <v>2</v>
+      </c>
+      <c r="F480" t="n">
+        <v>0</v>
+      </c>
+      <c r="G480" t="n">
+        <v>2</v>
+      </c>
+      <c r="H480" t="n">
+        <v>1</v>
+      </c>
+      <c r="I480" t="n">
+        <v>0</v>
+      </c>
+      <c r="J480" t="n">
+        <v>22</v>
+      </c>
+      <c r="K480" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="1" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B481" t="n">
+        <v>0</v>
+      </c>
+      <c r="C481" t="n">
+        <v>2</v>
+      </c>
+      <c r="D481" t="n">
+        <v>6</v>
+      </c>
+      <c r="E481" t="n">
+        <v>2</v>
+      </c>
+      <c r="F481" t="n">
+        <v>0</v>
+      </c>
+      <c r="G481" t="n">
+        <v>2</v>
+      </c>
+      <c r="H481" t="n">
+        <v>1</v>
+      </c>
+      <c r="I481" t="n">
+        <v>0</v>
+      </c>
+      <c r="J481" t="n">
+        <v>19</v>
+      </c>
+      <c r="K481" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="1" t="n">
+        <v>44396</v>
+      </c>
+      <c r="B482" t="n">
+        <v>0</v>
+      </c>
+      <c r="C482" t="n">
+        <v>2</v>
+      </c>
+      <c r="D482" t="n">
+        <v>6</v>
+      </c>
+      <c r="E482" t="n">
+        <v>2</v>
+      </c>
+      <c r="F482" t="n">
+        <v>0</v>
+      </c>
+      <c r="G482" t="n">
+        <v>2</v>
+      </c>
+      <c r="H482" t="n">
+        <v>1</v>
+      </c>
+      <c r="I482" t="n">
+        <v>0</v>
+      </c>
+      <c r="J482" t="n">
+        <v>21</v>
+      </c>
+      <c r="K482" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="1" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B483" t="n">
+        <v>0</v>
+      </c>
+      <c r="C483" t="n">
+        <v>1</v>
+      </c>
+      <c r="D483" t="n">
+        <v>5</v>
+      </c>
+      <c r="E483" t="n">
+        <v>2</v>
+      </c>
+      <c r="F483" t="n">
+        <v>0</v>
+      </c>
+      <c r="G483" t="n">
+        <v>2</v>
+      </c>
+      <c r="H483" t="n">
+        <v>0</v>
+      </c>
+      <c r="I483" t="n">
+        <v>0</v>
+      </c>
+      <c r="J483" t="n">
+        <v>29</v>
+      </c>
+      <c r="K483" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="1" t="n">
+        <v>44398</v>
+      </c>
+      <c r="B484" t="n">
+        <v>0</v>
+      </c>
+      <c r="C484" t="n">
+        <v>1</v>
+      </c>
+      <c r="D484" t="n">
+        <v>4</v>
+      </c>
+      <c r="E484" t="n">
+        <v>2</v>
+      </c>
+      <c r="F484" t="n">
+        <v>0</v>
+      </c>
+      <c r="G484" t="n">
+        <v>3</v>
+      </c>
+      <c r="H484" t="n">
+        <v>0</v>
+      </c>
+      <c r="I484" t="n">
+        <v>0</v>
+      </c>
+      <c r="J484" t="n">
+        <v>21</v>
+      </c>
+      <c r="K484" t="n">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -83577,7 +84977,7 @@
         <v>44388</v>
       </c>
       <c r="B467" t="n">
-        <v>8069</v>
+        <v>18069</v>
       </c>
       <c r="C467" t="n">
         <v>39296</v>
@@ -83605,6 +85005,356 @@
       </c>
       <c r="K467" t="n">
         <v>638889</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="1" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B468" t="n">
+        <v>18069</v>
+      </c>
+      <c r="C468" t="n">
+        <v>39296</v>
+      </c>
+      <c r="D468" t="n">
+        <v>108334</v>
+      </c>
+      <c r="E468" t="n">
+        <v>115311</v>
+      </c>
+      <c r="F468" t="n">
+        <v>48555</v>
+      </c>
+      <c r="G468" t="n">
+        <v>77419</v>
+      </c>
+      <c r="H468" t="n">
+        <v>63208</v>
+      </c>
+      <c r="I468" t="n">
+        <v>30466</v>
+      </c>
+      <c r="J468" t="n">
+        <v>138307</v>
+      </c>
+      <c r="K468" t="n">
+        <v>638965</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="1" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B469" t="n">
+        <v>18074</v>
+      </c>
+      <c r="C469" t="n">
+        <v>39293</v>
+      </c>
+      <c r="D469" t="n">
+        <v>108355</v>
+      </c>
+      <c r="E469" t="n">
+        <v>115320</v>
+      </c>
+      <c r="F469" t="n">
+        <v>48554</v>
+      </c>
+      <c r="G469" t="n">
+        <v>77422</v>
+      </c>
+      <c r="H469" t="n">
+        <v>63213</v>
+      </c>
+      <c r="I469" t="n">
+        <v>30473</v>
+      </c>
+      <c r="J469" t="n">
+        <v>138331</v>
+      </c>
+      <c r="K469" t="n">
+        <v>639035</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="1" t="n">
+        <v>44391</v>
+      </c>
+      <c r="B470" t="n">
+        <v>18079</v>
+      </c>
+      <c r="C470" t="n">
+        <v>39336</v>
+      </c>
+      <c r="D470" t="n">
+        <v>108365</v>
+      </c>
+      <c r="E470" t="n">
+        <v>115326</v>
+      </c>
+      <c r="F470" t="n">
+        <v>48555</v>
+      </c>
+      <c r="G470" t="n">
+        <v>77424</v>
+      </c>
+      <c r="H470" t="n">
+        <v>63221</v>
+      </c>
+      <c r="I470" t="n">
+        <v>30476</v>
+      </c>
+      <c r="J470" t="n">
+        <v>138372</v>
+      </c>
+      <c r="K470" t="n">
+        <v>639154</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="1" t="n">
+        <v>44392</v>
+      </c>
+      <c r="B471" t="n">
+        <v>18081</v>
+      </c>
+      <c r="C471" t="n">
+        <v>39337</v>
+      </c>
+      <c r="D471" t="n">
+        <v>108380</v>
+      </c>
+      <c r="E471" t="n">
+        <v>115335</v>
+      </c>
+      <c r="F471" t="n">
+        <v>48559</v>
+      </c>
+      <c r="G471" t="n">
+        <v>77433</v>
+      </c>
+      <c r="H471" t="n">
+        <v>63224</v>
+      </c>
+      <c r="I471" t="n">
+        <v>30482</v>
+      </c>
+      <c r="J471" t="n">
+        <v>138408</v>
+      </c>
+      <c r="K471" t="n">
+        <v>639239</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="1" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B472" t="n">
+        <v>18081</v>
+      </c>
+      <c r="C472" t="n">
+        <v>39340</v>
+      </c>
+      <c r="D472" t="n">
+        <v>108403</v>
+      </c>
+      <c r="E472" t="n">
+        <v>115343</v>
+      </c>
+      <c r="F472" t="n">
+        <v>48558</v>
+      </c>
+      <c r="G472" t="n">
+        <v>77441</v>
+      </c>
+      <c r="H472" t="n">
+        <v>63236</v>
+      </c>
+      <c r="I472" t="n">
+        <v>30484</v>
+      </c>
+      <c r="J472" t="n">
+        <v>138466</v>
+      </c>
+      <c r="K472" t="n">
+        <v>639352</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="1" t="n">
+        <v>44394</v>
+      </c>
+      <c r="B473" t="n">
+        <v>18083</v>
+      </c>
+      <c r="C473" t="n">
+        <v>39346</v>
+      </c>
+      <c r="D473" t="n">
+        <v>108421</v>
+      </c>
+      <c r="E473" t="n">
+        <v>115366</v>
+      </c>
+      <c r="F473" t="n">
+        <v>48509</v>
+      </c>
+      <c r="G473" t="n">
+        <v>77446</v>
+      </c>
+      <c r="H473" t="n">
+        <v>63246</v>
+      </c>
+      <c r="I473" t="n">
+        <v>30485</v>
+      </c>
+      <c r="J473" t="n">
+        <v>138520</v>
+      </c>
+      <c r="K473" t="n">
+        <v>639422</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="1" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B474" t="n">
+        <v>18084</v>
+      </c>
+      <c r="C474" t="n">
+        <v>39352</v>
+      </c>
+      <c r="D474" t="n">
+        <v>108448</v>
+      </c>
+      <c r="E474" t="n">
+        <v>115390</v>
+      </c>
+      <c r="F474" t="n">
+        <v>48543</v>
+      </c>
+      <c r="G474" t="n">
+        <v>77457</v>
+      </c>
+      <c r="H474" t="n">
+        <v>63250</v>
+      </c>
+      <c r="I474" t="n">
+        <v>30488</v>
+      </c>
+      <c r="J474" t="n">
+        <v>138561</v>
+      </c>
+      <c r="K474" t="n">
+        <v>639573</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="1" t="n">
+        <v>44396</v>
+      </c>
+      <c r="B475" t="n">
+        <v>18085</v>
+      </c>
+      <c r="C475" t="n">
+        <v>39370</v>
+      </c>
+      <c r="D475" t="n">
+        <v>108465</v>
+      </c>
+      <c r="E475" t="n">
+        <v>115417</v>
+      </c>
+      <c r="F475" t="n">
+        <v>48546</v>
+      </c>
+      <c r="G475" t="n">
+        <v>77465</v>
+      </c>
+      <c r="H475" t="n">
+        <v>63262</v>
+      </c>
+      <c r="I475" t="n">
+        <v>30488</v>
+      </c>
+      <c r="J475" t="n">
+        <v>138602</v>
+      </c>
+      <c r="K475" t="n">
+        <v>639700</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="1" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B476" t="n">
+        <v>18086</v>
+      </c>
+      <c r="C476" t="n">
+        <v>39379</v>
+      </c>
+      <c r="D476" t="n">
+        <v>108485</v>
+      </c>
+      <c r="E476" t="n">
+        <v>115441</v>
+      </c>
+      <c r="F476" t="n">
+        <v>48551</v>
+      </c>
+      <c r="G476" t="n">
+        <v>77478</v>
+      </c>
+      <c r="H476" t="n">
+        <v>63273</v>
+      </c>
+      <c r="I476" t="n">
+        <v>30495</v>
+      </c>
+      <c r="J476" t="n">
+        <v>138643</v>
+      </c>
+      <c r="K476" t="n">
+        <v>639831</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="1" t="n">
+        <v>44398</v>
+      </c>
+      <c r="B477" t="n">
+        <v>18092</v>
+      </c>
+      <c r="C477" t="n">
+        <v>39381</v>
+      </c>
+      <c r="D477" t="n">
+        <v>108511</v>
+      </c>
+      <c r="E477" t="n">
+        <v>115463</v>
+      </c>
+      <c r="F477" t="n">
+        <v>48558</v>
+      </c>
+      <c r="G477" t="n">
+        <v>77507</v>
+      </c>
+      <c r="H477" t="n">
+        <v>63293</v>
+      </c>
+      <c r="I477" t="n">
+        <v>30503</v>
+      </c>
+      <c r="J477" t="n">
+        <v>138710</v>
+      </c>
+      <c r="K477" t="n">
+        <v>640018</v>
       </c>
     </row>
   </sheetData>
@@ -100741,6 +102491,356 @@
         <v>10723</v>
       </c>
     </row>
+    <row r="490">
+      <c r="A490" s="1" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B490" t="n">
+        <v>343</v>
+      </c>
+      <c r="C490" t="n">
+        <v>821</v>
+      </c>
+      <c r="D490" t="n">
+        <v>1822</v>
+      </c>
+      <c r="E490" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F490" t="n">
+        <v>586</v>
+      </c>
+      <c r="G490" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H490" t="n">
+        <v>635</v>
+      </c>
+      <c r="I490" t="n">
+        <v>308</v>
+      </c>
+      <c r="J490" t="n">
+        <v>2360</v>
+      </c>
+      <c r="K490" t="n">
+        <v>10723</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="1" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B491" t="n">
+        <v>343</v>
+      </c>
+      <c r="C491" t="n">
+        <v>822</v>
+      </c>
+      <c r="D491" t="n">
+        <v>1822</v>
+      </c>
+      <c r="E491" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F491" t="n">
+        <v>586</v>
+      </c>
+      <c r="G491" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H491" t="n">
+        <v>635</v>
+      </c>
+      <c r="I491" t="n">
+        <v>308</v>
+      </c>
+      <c r="J491" t="n">
+        <v>2360</v>
+      </c>
+      <c r="K491" t="n">
+        <v>10724</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="1" t="n">
+        <v>44391</v>
+      </c>
+      <c r="B492" t="n">
+        <v>343</v>
+      </c>
+      <c r="C492" t="n">
+        <v>822</v>
+      </c>
+      <c r="D492" t="n">
+        <v>1822</v>
+      </c>
+      <c r="E492" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F492" t="n">
+        <v>587</v>
+      </c>
+      <c r="G492" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H492" t="n">
+        <v>635</v>
+      </c>
+      <c r="I492" t="n">
+        <v>308</v>
+      </c>
+      <c r="J492" t="n">
+        <v>2361</v>
+      </c>
+      <c r="K492" t="n">
+        <v>10726</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="1" t="n">
+        <v>44392</v>
+      </c>
+      <c r="B493" t="n">
+        <v>343</v>
+      </c>
+      <c r="C493" t="n">
+        <v>822</v>
+      </c>
+      <c r="D493" t="n">
+        <v>1822</v>
+      </c>
+      <c r="E493" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F493" t="n">
+        <v>588</v>
+      </c>
+      <c r="G493" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H493" t="n">
+        <v>635</v>
+      </c>
+      <c r="I493" t="n">
+        <v>308</v>
+      </c>
+      <c r="J493" t="n">
+        <v>2361</v>
+      </c>
+      <c r="K493" t="n">
+        <v>10727</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="1" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B494" t="n">
+        <v>343</v>
+      </c>
+      <c r="C494" t="n">
+        <v>822</v>
+      </c>
+      <c r="D494" t="n">
+        <v>1823</v>
+      </c>
+      <c r="E494" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F494" t="n">
+        <v>588</v>
+      </c>
+      <c r="G494" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H494" t="n">
+        <v>635</v>
+      </c>
+      <c r="I494" t="n">
+        <v>308</v>
+      </c>
+      <c r="J494" t="n">
+        <v>2361</v>
+      </c>
+      <c r="K494" t="n">
+        <v>10728</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="1" t="n">
+        <v>44394</v>
+      </c>
+      <c r="B495" t="n">
+        <v>343</v>
+      </c>
+      <c r="C495" t="n">
+        <v>822</v>
+      </c>
+      <c r="D495" t="n">
+        <v>1823</v>
+      </c>
+      <c r="E495" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F495" t="n">
+        <v>588</v>
+      </c>
+      <c r="G495" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H495" t="n">
+        <v>635</v>
+      </c>
+      <c r="I495" t="n">
+        <v>308</v>
+      </c>
+      <c r="J495" t="n">
+        <v>2361</v>
+      </c>
+      <c r="K495" t="n">
+        <v>10728</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="1" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B496" t="n">
+        <v>343</v>
+      </c>
+      <c r="C496" t="n">
+        <v>822</v>
+      </c>
+      <c r="D496" t="n">
+        <v>1824</v>
+      </c>
+      <c r="E496" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F496" t="n">
+        <v>588</v>
+      </c>
+      <c r="G496" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H496" t="n">
+        <v>635</v>
+      </c>
+      <c r="I496" t="n">
+        <v>308</v>
+      </c>
+      <c r="J496" t="n">
+        <v>2361</v>
+      </c>
+      <c r="K496" t="n">
+        <v>10729</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="1" t="n">
+        <v>44396</v>
+      </c>
+      <c r="B497" t="n">
+        <v>343</v>
+      </c>
+      <c r="C497" t="n">
+        <v>822</v>
+      </c>
+      <c r="D497" t="n">
+        <v>1824</v>
+      </c>
+      <c r="E497" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F497" t="n">
+        <v>588</v>
+      </c>
+      <c r="G497" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H497" t="n">
+        <v>635</v>
+      </c>
+      <c r="I497" t="n">
+        <v>308</v>
+      </c>
+      <c r="J497" t="n">
+        <v>2361</v>
+      </c>
+      <c r="K497" t="n">
+        <v>10729</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="1" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B498" t="n">
+        <v>343</v>
+      </c>
+      <c r="C498" t="n">
+        <v>822</v>
+      </c>
+      <c r="D498" t="n">
+        <v>1824</v>
+      </c>
+      <c r="E498" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F498" t="n">
+        <v>588</v>
+      </c>
+      <c r="G498" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H498" t="n">
+        <v>635</v>
+      </c>
+      <c r="I498" t="n">
+        <v>308</v>
+      </c>
+      <c r="J498" t="n">
+        <v>2361</v>
+      </c>
+      <c r="K498" t="n">
+        <v>10729</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="1" t="n">
+        <v>44398</v>
+      </c>
+      <c r="B499" t="n">
+        <v>343</v>
+      </c>
+      <c r="C499" t="n">
+        <v>822</v>
+      </c>
+      <c r="D499" t="n">
+        <v>1824</v>
+      </c>
+      <c r="E499" t="n">
+        <v>1757</v>
+      </c>
+      <c r="F499" t="n">
+        <v>588</v>
+      </c>
+      <c r="G499" t="n">
+        <v>2091</v>
+      </c>
+      <c r="H499" t="n">
+        <v>635</v>
+      </c>
+      <c r="I499" t="n">
+        <v>308</v>
+      </c>
+      <c r="J499" t="n">
+        <v>2361</v>
+      </c>
+      <c r="K499" t="n">
+        <v>10729</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>